<commit_message>
Change on CardLogic of Zhouzhou
</commit_message>
<xml_diff>
--- a/My project/Luban/Config/Datas/PlayerInfo.xlsx
+++ b/My project/Luban/Config/Datas/PlayerInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lofnh\Documents\GitHub\Draconia\My project\Luban\Config\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65B5572-E863-468C-B623-332637A5E888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB201FE-0E3F-4FDC-ADA2-DF2CAA28B30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="7485" windowWidth="28740" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="5625" windowWidth="28740" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>##</t>
   </si>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Passives</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HitDecreaseRate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -190,10 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>被动（暂时未添加）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>list#sep=|,int#ref=TbCardInfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -255,6 +247,38 @@
   </si>
   <si>
     <t>103|108|109|110|107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PassiveDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被动描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>避柳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场上有单位进入危险区时减少自身*PassiveModifier*费用。一次行动只能触发一次。（直到下个回合无法触发）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PassiveModifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被动数值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -581,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -592,7 +616,7 @@
     <col min="17" max="17" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -645,25 +669,31 @@
         <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
-        <v>22</v>
-      </c>
       <c r="U1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" t="s">
         <v>52</v>
       </c>
-      <c r="W1" t="s">
-        <v>54</v>
+      <c r="X1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -674,67 +704,73 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
       </c>
       <c r="U2" t="s">
         <v>5</v>
       </c>
       <c r="V2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="X2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -742,75 +778,81 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>35</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>36</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>37</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" t="s">
-        <v>39</v>
-      </c>
       <c r="R3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" t="s">
         <v>46</v>
       </c>
-      <c r="S3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" t="s">
-        <v>25</v>
-      </c>
-      <c r="U3" t="s">
-        <v>48</v>
-      </c>
       <c r="V3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" t="s">
         <v>53</v>
       </c>
-      <c r="W3" t="s">
-        <v>55</v>
+      <c r="X3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>10001</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -852,19 +894,19 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V4">
         <v>3</v>
@@ -872,13 +914,19 @@
       <c r="W4">
         <v>3</v>
       </c>
+      <c r="X4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>10002</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -920,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -932,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V5">
         <v>3</v>

</xml_diff>